<commit_message>
Updated with new output spreadsheet
</commit_message>
<xml_diff>
--- a/weight_adjusted_dk_by_category.xlsx
+++ b/weight_adjusted_dk_by_category.xlsx
@@ -978,22 +978,22 @@
         <v>0.0261636603843753</v>
       </c>
       <c r="I10">
-        <v>0.03441115048558141</v>
+        <v>0.0344111504855814</v>
       </c>
       <c r="J10">
-        <v>0.02786742912473334</v>
+        <v>0.02786742912473333</v>
       </c>
       <c r="K10">
-        <v>0.03161562274431219</v>
+        <v>0.03161562274431218</v>
       </c>
       <c r="L10">
-        <v>0.03110415048997383</v>
+        <v>0.03110415048997382</v>
       </c>
       <c r="M10">
         <v>0.02944040152524149</v>
       </c>
       <c r="N10">
-        <v>0.0591619175719514</v>
+        <v>0.05916191757195138</v>
       </c>
       <c r="O10">
         <v>0.04473869282723608</v>
@@ -1412,22 +1412,22 @@
         <v>0.02544844543324715</v>
       </c>
       <c r="I17">
-        <v>0.02945757253000238</v>
+        <v>0.02945757253000232</v>
       </c>
       <c r="J17">
-        <v>0.03291889070983222</v>
+        <v>0.03291889070983216</v>
       </c>
       <c r="K17">
-        <v>0.03292906357737031</v>
+        <v>0.03292906357737025</v>
       </c>
       <c r="L17">
-        <v>0.03312896042449348</v>
+        <v>0.03312896042449341</v>
       </c>
       <c r="M17">
-        <v>0.03699210687207728</v>
+        <v>0.0369921068720772</v>
       </c>
       <c r="N17">
-        <v>0.06446851344903964</v>
+        <v>0.06446851344903952</v>
       </c>
       <c r="O17">
         <v>0.03893970236224157</v>
@@ -1846,22 +1846,22 @@
         <v>0.03547875490980839</v>
       </c>
       <c r="I24">
-        <v>0.04024023400455259</v>
+        <v>0.04024023400455255</v>
       </c>
       <c r="J24">
-        <v>0.03619691449671982</v>
+        <v>0.03619691449671979</v>
       </c>
       <c r="K24">
-        <v>0.0333354182583212</v>
+        <v>0.03333541825832117</v>
       </c>
       <c r="L24">
-        <v>0.03742963694703171</v>
+        <v>0.03742963694703168</v>
       </c>
       <c r="M24">
-        <v>0.03117055707760708</v>
+        <v>0.03117055707760705</v>
       </c>
       <c r="N24">
-        <v>0.06906917553202947</v>
+        <v>0.0690691755320294</v>
       </c>
       <c r="O24">
         <v>0.04799083713452296</v>
@@ -2280,22 +2280,22 @@
         <v>0.04890286315705822</v>
       </c>
       <c r="I31">
-        <v>0.03828325707994967</v>
+        <v>0.03828325707994965</v>
       </c>
       <c r="J31">
-        <v>0.03805248467503126</v>
+        <v>0.03805248467503123</v>
       </c>
       <c r="K31">
-        <v>0.03765716594166098</v>
+        <v>0.03765716594166096</v>
       </c>
       <c r="L31">
-        <v>0.04457473434428293</v>
+        <v>0.0445747343442829</v>
       </c>
       <c r="M31">
-        <v>0.03884872588670352</v>
+        <v>0.0388487258867035</v>
       </c>
       <c r="N31">
-        <v>0.07970563018441935</v>
+        <v>0.0797056301844193</v>
       </c>
       <c r="O31">
         <v>0.05194111177280585</v>
@@ -2714,22 +2714,22 @@
         <v>0.05162622339919293</v>
       </c>
       <c r="I38">
-        <v>0.04347079461927138</v>
+        <v>0.04347079461927145</v>
       </c>
       <c r="J38">
-        <v>0.0504074085334675</v>
+        <v>0.05040740853346758</v>
       </c>
       <c r="K38">
-        <v>0.03976947788541872</v>
+        <v>0.03976947788541878</v>
       </c>
       <c r="L38">
-        <v>0.0572226355221518</v>
+        <v>0.05722263552215189</v>
       </c>
       <c r="M38">
-        <v>0.04252079224918554</v>
+        <v>0.04252079224918561</v>
       </c>
       <c r="N38">
-        <v>0.08920556677815386</v>
+        <v>0.089205566778154</v>
       </c>
       <c r="O38">
         <v>0.05596061216476105</v>
@@ -3086,22 +3086,22 @@
         <v>0.05772527537400176</v>
       </c>
       <c r="I44">
-        <v>0.05168854234797064</v>
+        <v>0.05168854234797048</v>
       </c>
       <c r="J44">
-        <v>0.05506446794882901</v>
+        <v>0.05506446794882883</v>
       </c>
       <c r="K44">
-        <v>0.05819475666640396</v>
+        <v>0.05819475666640378</v>
       </c>
       <c r="L44">
-        <v>0.0534098020082959</v>
+        <v>0.05340980200829573</v>
       </c>
       <c r="M44">
-        <v>0.05302261734395435</v>
+        <v>0.05302261734395418</v>
       </c>
       <c r="N44">
-        <v>0.09422365921244659</v>
+        <v>0.0942236592124463</v>
       </c>
       <c r="O44">
         <v>0.0612619795957861</v>
@@ -3496,22 +3496,22 @@
         <v>0.02952712280291519</v>
       </c>
       <c r="I51">
-        <v>0.0335009105790027</v>
+        <v>0.03350091057900279</v>
       </c>
       <c r="J51">
-        <v>0.03953075799870746</v>
+        <v>0.03953075799870756</v>
       </c>
       <c r="K51">
-        <v>0.04680130577649616</v>
+        <v>0.04680130577649628</v>
       </c>
       <c r="L51">
-        <v>0.05130392005266703</v>
+        <v>0.05130392005266715</v>
       </c>
       <c r="M51">
-        <v>0.04884718964602951</v>
+        <v>0.04884718964602963</v>
       </c>
       <c r="N51">
-        <v>0.07308700282151315</v>
+        <v>0.07308700282151333</v>
       </c>
       <c r="O51">
         <v>0.02735433137481898</v>
@@ -4240,22 +4240,22 @@
         <v>0.01645959162905423</v>
       </c>
       <c r="I63">
-        <v>0.04552762445813475</v>
+        <v>0.04552762445813478</v>
       </c>
       <c r="J63">
-        <v>0.03691426930207466</v>
+        <v>0.03691426930207468</v>
       </c>
       <c r="K63">
-        <v>0.04071339519503274</v>
+        <v>0.04071339519503276</v>
       </c>
       <c r="L63">
-        <v>0.04117344155465967</v>
+        <v>0.0411734415546597</v>
       </c>
       <c r="M63">
-        <v>0.04347895485537848</v>
+        <v>0.0434789548553785</v>
       </c>
       <c r="N63">
-        <v>0.02761712827272828</v>
+        <v>0.02761712827272829</v>
       </c>
       <c r="O63">
         <v>0.05265937073087196</v>
@@ -4881,7 +4881,7 @@
         <v>0.05081340193959259</v>
       </c>
       <c r="E10">
-        <v>0.1083135227309886</v>
+        <v>0.1083135227309885</v>
       </c>
       <c r="F10">
         <v>0.1052871492108051</v>
@@ -5063,10 +5063,10 @@
         <v>0.0564085504986231</v>
       </c>
       <c r="E17">
-        <v>0.1102001308230767</v>
+        <v>0.1102001308230765</v>
       </c>
       <c r="F17">
-        <v>0.1196949767397385</v>
+        <v>0.1196949767397383</v>
       </c>
       <c r="G17">
         <v>0.1609347644523384</v>
@@ -5245,10 +5245,10 @@
         <v>0.07460629736820848</v>
       </c>
       <c r="E24">
-        <v>0.1213540296324396</v>
+        <v>0.1213540296324395</v>
       </c>
       <c r="F24">
-        <v>0.1260879066838222</v>
+        <v>0.1260879066838221</v>
       </c>
       <c r="G24">
         <v>0.166909809437012</v>
@@ -5427,10 +5427,10 @@
         <v>0.09009701101339665</v>
       </c>
       <c r="E31">
-        <v>0.1410742786579338</v>
+        <v>0.1410742786579337</v>
       </c>
       <c r="F31">
-        <v>0.1360477194541139</v>
+        <v>0.1360477194541138</v>
       </c>
       <c r="G31">
         <v>0.2094211178656051</v>
@@ -5609,10 +5609,10 @@
         <v>0.08986341695832241</v>
       </c>
       <c r="E38">
-        <v>0.1744587738875957</v>
+        <v>0.174458773887596</v>
       </c>
       <c r="F38">
-        <v>0.1481379017000529</v>
+        <v>0.1481379017000531</v>
       </c>
       <c r="G38">
         <v>0.2210740794291416</v>
@@ -5765,10 +5765,10 @@
         <v>0.1021450450164439</v>
       </c>
       <c r="E44">
-        <v>0.2043829074363588</v>
+        <v>0.2043829074363581</v>
       </c>
       <c r="F44">
-        <v>0.1612209380915414</v>
+        <v>0.1612209380915409</v>
       </c>
       <c r="G44">
         <v>0.2426836227248018</v>
@@ -5944,10 +5944,10 @@
         <v>0.07093414308730633</v>
       </c>
       <c r="E51">
-        <v>0.1535435980469124</v>
+        <v>0.1535435980469128</v>
       </c>
       <c r="F51">
-        <v>0.1395274888275033</v>
+        <v>0.1395274888275036</v>
       </c>
       <c r="G51">
         <v>0.1432400798835881</v>
@@ -6256,10 +6256,10 @@
         <v>0.08647598745967557</v>
       </c>
       <c r="E63">
-        <v>0.09527948065550836</v>
+        <v>0.09527948065550843</v>
       </c>
       <c r="F63">
-        <v>0.1401453329825</v>
+        <v>0.1401453329825001</v>
       </c>
       <c r="G63">
         <v>0.08985179832897647</v>
@@ -6792,7 +6792,7 @@
         <v>0.01782100130454707</v>
       </c>
       <c r="F10">
-        <v>0.03607001898987159</v>
+        <v>0.03607001898987158</v>
       </c>
       <c r="G10">
         <v>0.04366303934578403</v>
@@ -7091,16 +7091,16 @@
         <v>41000</v>
       </c>
       <c r="C17">
-        <v>0.01043787073744136</v>
+        <v>0.01043787073744134</v>
       </c>
       <c r="D17">
-        <v>0.02306545121245325</v>
+        <v>0.0230654512124532</v>
       </c>
       <c r="E17">
-        <v>0.02295711017317276</v>
+        <v>0.02295711017317271</v>
       </c>
       <c r="F17">
-        <v>0.05014613324218452</v>
+        <v>0.05014613324218441</v>
       </c>
       <c r="G17">
         <v>0.03247789690205662</v>
@@ -7399,16 +7399,16 @@
         <v>41640</v>
       </c>
       <c r="C24">
-        <v>0.0236334266316163</v>
+        <v>0.02363342663161628</v>
       </c>
       <c r="D24">
-        <v>0.03395532470005568</v>
+        <v>0.03395532470005565</v>
       </c>
       <c r="E24">
-        <v>0.02551846893238083</v>
+        <v>0.02551846893238081</v>
       </c>
       <c r="F24">
-        <v>0.06215701612288535</v>
+        <v>0.06215701612288529</v>
       </c>
       <c r="G24">
         <v>0.0529371739508628</v>
@@ -7707,16 +7707,16 @@
         <v>42278</v>
       </c>
       <c r="C31">
-        <v>0.02139866416909456</v>
+        <v>0.02139866416909454</v>
       </c>
       <c r="D31">
-        <v>0.04496597762679372</v>
+        <v>0.04496597762679368</v>
       </c>
       <c r="E31">
-        <v>0.03601475924528768</v>
+        <v>0.03601475924528766</v>
       </c>
       <c r="F31">
-        <v>0.07801482750908965</v>
+        <v>0.07801482750908961</v>
       </c>
       <c r="G31">
         <v>0.04376219132917266</v>
@@ -8015,16 +8015,16 @@
         <v>42917</v>
       </c>
       <c r="C38">
-        <v>0.02937204771056788</v>
+        <v>0.02937204771056793</v>
       </c>
       <c r="D38">
-        <v>0.04505173257072564</v>
+        <v>0.04505173257072571</v>
       </c>
       <c r="E38">
-        <v>0.04976070339128622</v>
+        <v>0.0497607033912863</v>
       </c>
       <c r="F38">
-        <v>0.07108615342703746</v>
+        <v>0.07108615342703757</v>
       </c>
       <c r="G38">
         <v>0.06489991211517315</v>
@@ -8279,16 +8279,16 @@
         <v>43466</v>
       </c>
       <c r="C44">
-        <v>0.03988386899589564</v>
+        <v>0.03988386899589551</v>
       </c>
       <c r="D44">
-        <v>0.05589107042511225</v>
+        <v>0.05589107042511207</v>
       </c>
       <c r="E44">
-        <v>0.05534407366798751</v>
+        <v>0.05534407366798734</v>
       </c>
       <c r="F44">
-        <v>0.06892541826744322</v>
+        <v>0.068925418267443</v>
       </c>
       <c r="G44">
         <v>0.06872263526140532</v>
@@ -8578,16 +8578,16 @@
         <v>44105</v>
       </c>
       <c r="C51">
-        <v>0.02515858548417828</v>
+        <v>0.02515858548417834</v>
       </c>
       <c r="D51">
-        <v>0.03893102667202124</v>
+        <v>0.03893102667202133</v>
       </c>
       <c r="E51">
-        <v>0.03435963370767028</v>
+        <v>0.03435963370767037</v>
       </c>
       <c r="F51">
-        <v>0.05441103615732173</v>
+        <v>0.05441103615732187</v>
       </c>
       <c r="G51">
         <v>0.05791081118532845</v>
@@ -9106,16 +9106,16 @@
         <v>45200</v>
       </c>
       <c r="C63">
-        <v>0.02940317876148385</v>
+        <v>0.02940317876148387</v>
       </c>
       <c r="D63">
-        <v>0.03980296819136622</v>
+        <v>0.03980296819136624</v>
       </c>
       <c r="E63">
-        <v>0.02698906665018333</v>
+        <v>0.02698906665018334</v>
       </c>
       <c r="F63">
-        <v>0.04423413692415437</v>
+        <v>0.0442341369241544</v>
       </c>
       <c r="G63">
         <v>0.04989654597303035</v>
@@ -9930,13 +9930,13 @@
         <v>0.05840105378901866</v>
       </c>
       <c r="D10">
-        <v>0.00976921766707158</v>
+        <v>0.009769217667071584</v>
       </c>
       <c r="E10">
-        <v>0.009461260613171285</v>
+        <v>0.009461260613171289</v>
       </c>
       <c r="F10">
-        <v>0.004988806663975905</v>
+        <v>0.004988806663975906</v>
       </c>
       <c r="G10">
         <v>0.01001324068917958</v>
@@ -10298,19 +10298,19 @@
         <v>41000</v>
       </c>
       <c r="C17">
-        <v>0.0645020839119152</v>
+        <v>0.06450208391191534</v>
       </c>
       <c r="D17">
-        <v>0.007913982301245053</v>
+        <v>0.007913982301245069</v>
       </c>
       <c r="E17">
-        <v>0.01378779601772927</v>
+        <v>0.0137877960177293</v>
       </c>
       <c r="F17">
-        <v>0.004294984674575053</v>
+        <v>0.004294984674575061</v>
       </c>
       <c r="G17">
-        <v>0.01610771845978716</v>
+        <v>0.01610771845978719</v>
       </c>
       <c r="P17">
         <v>0.1335977261606479</v>
@@ -10669,19 +10669,19 @@
         <v>41640</v>
       </c>
       <c r="C24">
-        <v>0.08793833754158982</v>
+        <v>0.0879383375415899</v>
       </c>
       <c r="D24">
-        <v>0.02285322575458035</v>
+        <v>0.02285322575458037</v>
       </c>
       <c r="E24">
-        <v>0.01492586825519381</v>
+        <v>0.01492586825519382</v>
       </c>
       <c r="F24">
-        <v>0.005552315621515716</v>
+        <v>0.005552315621515721</v>
       </c>
       <c r="G24">
-        <v>0.0139944892140584</v>
+        <v>0.01399448921405841</v>
       </c>
       <c r="P24">
         <v>0.1407737131306973</v>
@@ -11040,19 +11040,19 @@
         <v>42278</v>
       </c>
       <c r="C31">
-        <v>0.1287974923750862</v>
+        <v>0.1287974923750863</v>
       </c>
       <c r="D31">
-        <v>0.01095786849844598</v>
+        <v>0.01095786849844599</v>
       </c>
       <c r="E31">
-        <v>0.01930082583917356</v>
+        <v>0.01930082583917357</v>
       </c>
       <c r="F31">
-        <v>0.007050529986912713</v>
+        <v>0.007050529986912717</v>
       </c>
       <c r="G31">
-        <v>0.01428751185064696</v>
+        <v>0.01428751185064697</v>
       </c>
       <c r="P31">
         <v>0.1808150188515076</v>
@@ -11465,22 +11465,22 @@
         <v>42917</v>
       </c>
       <c r="C38">
-        <v>0.1189640901503916</v>
+        <v>0.1189640901503914</v>
       </c>
       <c r="D38">
-        <v>0.01278613147198069</v>
+        <v>0.01278613147198067</v>
       </c>
       <c r="E38">
-        <v>0.02004488183133302</v>
+        <v>0.02004488183133299</v>
       </c>
       <c r="F38">
-        <v>0.01309016009300313</v>
+        <v>0.01309016009300311</v>
       </c>
       <c r="H38">
-        <v>0.0278567027924008</v>
+        <v>0.02785670279240076</v>
       </c>
       <c r="I38">
-        <v>0.002528670760508202</v>
+        <v>0.002528670760508199</v>
       </c>
       <c r="P38">
         <v>0.1767450166940215</v>
@@ -11837,22 +11837,22 @@
         <v>43466</v>
       </c>
       <c r="C44">
-        <v>0.1304551974884444</v>
+        <v>0.1304551974884448</v>
       </c>
       <c r="D44">
-        <v>0.01566846990331823</v>
+        <v>0.01566846990331828</v>
       </c>
       <c r="E44">
-        <v>0.02063609399446528</v>
+        <v>0.02063609399446534</v>
       </c>
       <c r="F44">
-        <v>0.01353981713030841</v>
+        <v>0.01353981713030845</v>
       </c>
       <c r="H44">
-        <v>0.03494805169080592</v>
+        <v>0.03494805169080602</v>
       </c>
       <c r="I44">
-        <v>0.004796801149095449</v>
+        <v>0.004796801149095463</v>
       </c>
       <c r="P44">
         <v>0.2056035923146081</v>
@@ -12247,22 +12247,22 @@
         <v>44105</v>
       </c>
       <c r="C51">
-        <v>0.04015210043639664</v>
+        <v>0.04015210043639654</v>
       </c>
       <c r="D51">
-        <v>0.01417126951007108</v>
+        <v>0.01417126951007104</v>
       </c>
       <c r="E51">
-        <v>0.02112177448436273</v>
+        <v>0.02112177448436268</v>
       </c>
       <c r="F51">
-        <v>0.02387570024470281</v>
+        <v>0.02387570024470275</v>
       </c>
       <c r="H51">
-        <v>0.04660423382848524</v>
+        <v>0.04660423382848512</v>
       </c>
       <c r="I51">
-        <v>0.006935203517173399</v>
+        <v>0.006935203517173381</v>
       </c>
       <c r="P51">
         <v>0.05566217503994367</v>
@@ -12994,19 +12994,19 @@
         <v>0.01024565585970226</v>
       </c>
       <c r="K63">
-        <v>0.03131766339118448</v>
+        <v>0.03131766339118446</v>
       </c>
       <c r="L63">
-        <v>0.04185583727103546</v>
+        <v>0.04185583727103544</v>
       </c>
       <c r="M63">
-        <v>0.01764032001010938</v>
+        <v>0.01764032001010937</v>
       </c>
       <c r="N63">
-        <v>0.02222108232261463</v>
+        <v>0.02222108232261462</v>
       </c>
       <c r="O63">
-        <v>0.0171487916725416</v>
+        <v>0.01714879167254158</v>
       </c>
       <c r="W63">
         <v>0.01659239124786226</v>
@@ -13872,19 +13872,19 @@
         <v>0.0766056592843195</v>
       </c>
       <c r="M10">
-        <v>0.01904941319783873</v>
+        <v>0.01904941319783874</v>
       </c>
       <c r="N10">
-        <v>0.06985207812445854</v>
+        <v>0.06985207812445857</v>
       </c>
       <c r="O10">
-        <v>0.04894955409673171</v>
+        <v>0.04894955409673172</v>
       </c>
       <c r="P10">
-        <v>0.04893149639309569</v>
+        <v>0.04893149639309571</v>
       </c>
       <c r="Q10">
-        <v>0.1049972498605408</v>
+        <v>0.1049972498605409</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -14243,19 +14243,19 @@
         <v>0.0675793763421827</v>
       </c>
       <c r="M17">
-        <v>0.0286361134763028</v>
+        <v>0.02863611347630286</v>
       </c>
       <c r="N17">
-        <v>0.08341242737844183</v>
+        <v>0.083412427378442</v>
       </c>
       <c r="O17">
-        <v>0.06310687512906824</v>
+        <v>0.06310687512906836</v>
       </c>
       <c r="P17">
-        <v>0.04557698978745827</v>
+        <v>0.04557698978745836</v>
       </c>
       <c r="Q17">
-        <v>0.1010832069354542</v>
+        <v>0.1010832069354544</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -14614,19 +14614,19 @@
         <v>0.08521383860097642</v>
       </c>
       <c r="M24">
-        <v>0.02350807790258909</v>
+        <v>0.02350807790258911</v>
       </c>
       <c r="N24">
-        <v>0.08285196467039735</v>
+        <v>0.08285196467039742</v>
       </c>
       <c r="O24">
-        <v>0.06889723252796981</v>
+        <v>0.06889723252796988</v>
       </c>
       <c r="P24">
-        <v>0.05296173723715698</v>
+        <v>0.05296173723715702</v>
       </c>
       <c r="Q24">
-        <v>0.1048892841524007</v>
+        <v>0.1048892841524008</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -14985,19 +14985,19 @@
         <v>0.09205220856323544</v>
       </c>
       <c r="M31">
-        <v>0.03705196148902712</v>
+        <v>0.03705196148902715</v>
       </c>
       <c r="N31">
-        <v>0.0860551826235003</v>
+        <v>0.08605518262350036</v>
       </c>
       <c r="O31">
-        <v>0.06984405796717537</v>
+        <v>0.06984405796717541</v>
       </c>
       <c r="P31">
-        <v>0.04624210317717056</v>
+        <v>0.04624210317717059</v>
       </c>
       <c r="Q31">
-        <v>0.1574560628189997</v>
+        <v>0.1574560628189998</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -15356,19 +15356,19 @@
         <v>0.08063181214623964</v>
       </c>
       <c r="M38">
-        <v>0.03201679385087261</v>
+        <v>0.03201679385087256</v>
       </c>
       <c r="N38">
-        <v>0.1073937062731937</v>
+        <v>0.1073937062731935</v>
       </c>
       <c r="O38">
-        <v>0.09164750566984002</v>
+        <v>0.09164750566983988</v>
       </c>
       <c r="P38">
-        <v>0.07070311097141897</v>
+        <v>0.07070311097141886</v>
       </c>
       <c r="Q38">
-        <v>0.09954479704936872</v>
+        <v>0.09954479704936857</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -15674,19 +15674,19 @@
         <v>0.1023852246052861</v>
       </c>
       <c r="M44">
-        <v>0.03194471287831606</v>
+        <v>0.03194471287831616</v>
       </c>
       <c r="N44">
-        <v>0.1199346169080686</v>
+        <v>0.1199346169080689</v>
       </c>
       <c r="O44">
-        <v>0.09044894830112932</v>
+        <v>0.09044894830112959</v>
       </c>
       <c r="P44">
-        <v>0.08190657382091909</v>
+        <v>0.08190657382091936</v>
       </c>
       <c r="Q44">
-        <v>0.116800667525748</v>
+        <v>0.1168006675257484</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -16027,19 +16027,19 @@
         <v>0.06827754018622374</v>
       </c>
       <c r="M51">
-        <v>0.01927300354644673</v>
+        <v>0.01927300354644668</v>
       </c>
       <c r="N51">
-        <v>0.07516591902239303</v>
+        <v>0.07516591902239285</v>
       </c>
       <c r="O51">
-        <v>0.08010118812335487</v>
+        <v>0.08010118812335468</v>
       </c>
       <c r="P51">
-        <v>0.03297693471641796</v>
+        <v>0.03297693471641788</v>
       </c>
       <c r="Q51">
-        <v>0.06759903153752772</v>
+        <v>0.06759903153752755</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -16663,19 +16663,19 @@
         <v>0.06309327418813286</v>
       </c>
       <c r="M63">
-        <v>0.01859929970012776</v>
+        <v>0.01859929970012775</v>
       </c>
       <c r="N63">
-        <v>0.06435563742367574</v>
+        <v>0.0643556374236757</v>
       </c>
       <c r="O63">
-        <v>0.05108974905681744</v>
+        <v>0.0510897490568174</v>
       </c>
       <c r="P63">
-        <v>0.03926904893631185</v>
+        <v>0.03926904893631182</v>
       </c>
       <c r="Q63">
-        <v>0.05581601598092315</v>
+        <v>0.05581601598092312</v>
       </c>
     </row>
     <row r="64" spans="1:17">

</xml_diff>